<commit_message>
change mapping, add mapping test to nols
</commit_message>
<xml_diff>
--- a/mapping/mapping_nols.xlsx
+++ b/mapping/mapping_nols.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\FO Bildrift\60 Analyse\Rapportmaler\08 Leaseplan kontering\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Nettverk Norge\Felles\Kontering LP\bildrift_lp_posting\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BADA60C2-246B-4B9B-A805-C089E5010949}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1660F475-7998-4980-8BB6-1A5F006FFF50}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3789B234-9D36-4C8B-BF65-5FBA0B4BEF1A}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{3789B234-9D36-4C8B-BF65-5FBA0B4BEF1A}"/>
   </bookViews>
   <sheets>
     <sheet name="Kontering" sheetId="1" r:id="rId1"/>
@@ -219,7 +219,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -319,7 +319,9 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="Invisible" pivot="0" table="0" count="0" xr9:uid="{F20FB33F-97A9-43EF-ABDB-6A04FEAD84B2}"/>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -647,7 +649,7 @@
   <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
+      <selection activeCell="J19" sqref="J19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>